<commit_message>
add load general config for cons-lay, add 2 objective prototypes - Risk adn Hoisting Time
</commit_message>
<xml_diff>
--- a/data/conslay/dynamic_locations.xlsx
+++ b/data/conslay/dynamic_locations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daovudat/Desktop/Projects/matlab/moaha-place-OBL/moaha_place_obl_3cases/multiphase/static/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daovudat/Desktop/Projects/freelance/golang-moaha-construction/data/conslay/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54808CE3-EC8F-1B4E-A77C-C12C02ED55AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D385C01B-9030-0A41-A1A8-6C98E5F1A4CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{82FBD6D4-541B-A340-931E-720121D87B31}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{82FBD6D4-541B-A340-931E-720121D87B31}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
   <si>
     <t>Symbol</t>
   </si>
@@ -76,15 +76,6 @@
   </si>
   <si>
     <t>TF7</t>
-  </si>
-  <si>
-    <t>TF8</t>
-  </si>
-  <si>
-    <t>TF9</t>
-  </si>
-  <si>
-    <t>TF10</t>
   </si>
   <si>
     <t>TF11</t>
@@ -477,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA024008-5D72-9649-81A4-DE7FF0B70DB1}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="E21" sqref="A15:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -626,10 +617,10 @@
         <v>13</v>
       </c>
       <c r="B9" s="3">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C9" s="3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>6</v>
@@ -643,7 +634,7 @@
         <v>14</v>
       </c>
       <c r="B10" s="3">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C10" s="3">
         <v>6</v>
@@ -655,56 +646,26 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="3">
-        <v>10</v>
-      </c>
-      <c r="C11" s="3">
-        <v>6</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="3">
-        <v>6</v>
-      </c>
-      <c r="C12" s="3">
-        <v>4</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="3">
-        <v>8</v>
-      </c>
-      <c r="C13" s="3">
-        <v>6</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>6</v>
-      </c>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>